<commit_message>
sparql rdf model of categories in test, generated py #61
</commit_message>
<xml_diff>
--- a/config/categories/GW portal list of icons new structure 20170830.xlsx
+++ b/config/categories/GW portal list of icons new structure 20170830.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magali\Desktop\SACportal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\build\sac-categories\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="907" activeTab="2"/>
+    <workbookView xWindow="1530" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="907"/>
   </bookViews>
   <sheets>
     <sheet name="science domain categories" sheetId="7" r:id="rId1"/>
     <sheet name="synonyms" sheetId="8" r:id="rId2"/>
     <sheet name="about" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -668,9 +668,6 @@
   </si>
   <si>
     <t>deniz-fuchidzhiev-249553.jpg</t>
-  </si>
-  <si>
-    <t>mike-toews-GNS-extrinsic2.pmg</t>
   </si>
   <si>
     <t>ruthie-163318.jpg</t>
@@ -788,6 +785,9 @@
       <t>, which aimed to develop a suite of innovative methods for rapid and cost-effective characterisation of New Zealand’s groundwater systems. 
 The SAC programme was funded by the Ministry of Business, Innovation &amp; Employment over the 2011-2017 period.</t>
     </r>
+  </si>
+  <si>
+    <t>mike-toews-GNS-extrinsic2.png</t>
   </si>
 </sst>
 </file>
@@ -1302,23 +1302,23 @@
   </sheetPr>
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="2" customWidth="1"/>
     <col min="2" max="2" width="46" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.73046875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.1328125" style="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
     <col min="9" max="9" width="25" style="1" customWidth="1"/>
-    <col min="10" max="1022" width="9.140625" style="1" customWidth="1"/>
-    <col min="1023" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="1022" width="9.1328125" style="1" customWidth="1"/>
+    <col min="1023" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1">
@@ -1355,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -1366,7 +1366,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="17"/>
       <c r="H2" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>33</v>
@@ -1377,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
@@ -1388,7 +1388,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="17"/>
       <c r="H3" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>34</v>
@@ -1412,10 +1412,10 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>35</v>
@@ -1439,7 +1439,7 @@
         <v>211</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>36</v>
@@ -1466,7 +1466,7 @@
         <v>210</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>37</v>
@@ -1490,10 +1490,10 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="17" t="s">
-        <v>214</v>
+        <v>244</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>38</v>
@@ -1504,7 +1504,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>1</v>
@@ -1517,7 +1517,7 @@
         <v>212</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>39</v>
@@ -1544,7 +1544,7 @@
         <v>213</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>40</v>
@@ -1580,7 +1580,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="17"/>
       <c r="H12" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>35</v>
@@ -1602,7 +1602,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="17"/>
       <c r="H13" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>36</v>
@@ -1624,7 +1624,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="17"/>
       <c r="H14" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>37</v>
@@ -1646,7 +1646,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="17"/>
       <c r="H15" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>38</v>
@@ -1671,7 +1671,7 @@
         <v>2.1</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1">
@@ -1713,7 +1713,7 @@
         <v>47</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>1</v>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1">
@@ -1734,7 +1734,7 @@
         <v>48</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>1</v>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>40</v>
@@ -1758,7 +1758,7 @@
         <v>49</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>1</v>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1">
@@ -1779,7 +1779,7 @@
         <v>50</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>1</v>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1">
@@ -1800,7 +1800,7 @@
         <v>51</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>1</v>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" customHeight="1">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1">
@@ -1918,7 +1918,7 @@
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1">
@@ -1926,7 +1926,7 @@
         <v>57</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>1</v>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="13" customFormat="1" ht="15" customHeight="1">
@@ -1982,7 +1982,7 @@
         <v>3.1</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>0</v>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="G34" s="17"/>
       <c r="H34" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1">
@@ -2006,7 +2006,7 @@
         <v>3.2</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>0</v>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="G35" s="17"/>
       <c r="H35" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1">
@@ -2030,7 +2030,7 @@
         <v>3.3</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
@@ -2046,7 +2046,7 @@
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1">
@@ -2054,7 +2054,7 @@
         <v>3.4</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="G37" s="17"/>
       <c r="H37" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="13" customFormat="1" ht="15" customHeight="1">
@@ -2091,7 +2091,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>0</v>
@@ -2104,7 +2104,7 @@
       </c>
       <c r="G40" s="17"/>
       <c r="H40" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1">
@@ -2125,7 +2125,7 @@
       </c>
       <c r="G41" s="17"/>
       <c r="H41" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="G42" s="17"/>
       <c r="H42" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="G43" s="17"/>
       <c r="H43" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="G44" s="17"/>
       <c r="H44" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="G45" s="17"/>
       <c r="H45" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="G46" s="17"/>
       <c r="H46" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="13" customFormat="1" ht="15" customHeight="1">
@@ -2266,7 +2266,7 @@
       </c>
       <c r="G49" s="17"/>
       <c r="H49" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="G51" s="17"/>
       <c r="H51" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1">
@@ -2322,7 +2322,7 @@
         <v>5.4</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
@@ -2338,7 +2338,7 @@
       </c>
       <c r="G52" s="17"/>
       <c r="H52" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15" customHeight="1">
@@ -2346,7 +2346,7 @@
         <v>5.5</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15" customHeight="1">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="G54" s="17"/>
       <c r="H54" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15" customHeight="1">
@@ -2394,7 +2394,7 @@
         <v>5.7</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="G55" s="17"/>
       <c r="H55" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15" customHeight="1">
@@ -2434,7 +2434,7 @@
       </c>
       <c r="G56" s="17"/>
       <c r="H56" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15" customHeight="1">
@@ -2458,7 +2458,7 @@
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="13" customFormat="1" ht="15" customHeight="1">
@@ -2494,7 +2494,7 @@
       </c>
       <c r="G60" s="17"/>
       <c r="H60" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15" customHeight="1">
@@ -2502,7 +2502,7 @@
         <v>63</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>0</v>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="G61" s="17"/>
       <c r="H61" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="15" customHeight="1">
@@ -2542,7 +2542,7 @@
       </c>
       <c r="G62" s="17"/>
       <c r="H62" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15" customHeight="1">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="G63" s="17"/>
       <c r="H63" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15" customHeight="1">
@@ -2590,7 +2590,7 @@
       </c>
       <c r="G64" s="17"/>
       <c r="H64" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15" customHeight="1">
@@ -2598,7 +2598,7 @@
         <v>67</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>0</v>
@@ -2614,7 +2614,7 @@
       </c>
       <c r="G65" s="17"/>
       <c r="H65" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="15" customHeight="1">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="G66" s="17"/>
       <c r="H66" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1">
@@ -2662,7 +2662,7 @@
       </c>
       <c r="G67" s="17"/>
       <c r="H67" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="13" customFormat="1" ht="15" customHeight="1">
@@ -2695,7 +2695,7 @@
       </c>
       <c r="G70" s="17"/>
       <c r="H70" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15" customHeight="1">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="G71" s="17"/>
       <c r="H71" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15" customHeight="1">
@@ -2737,7 +2737,7 @@
       </c>
       <c r="G72" s="17"/>
       <c r="H72" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="15" customHeight="1">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="G73" s="17"/>
       <c r="H73" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15" customHeight="1">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="G74" s="17"/>
       <c r="H74" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1">
@@ -2800,7 +2800,7 @@
       </c>
       <c r="G75" s="17"/>
       <c r="H75" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="13" customFormat="1" ht="15" customHeight="1">
@@ -2821,7 +2821,7 @@
         <v>158</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>0</v>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="G78" s="17"/>
       <c r="H78" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="15" customHeight="1">
@@ -2845,7 +2845,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>0</v>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="G79" s="17"/>
       <c r="H79" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="15" customHeight="1">
@@ -2869,7 +2869,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>0</v>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="G80" s="17"/>
       <c r="H80" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2909,11 +2909,11 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" style="1" customWidth="1"/>
     <col min="2" max="2" width="45" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2987,43 +2987,43 @@
   </sheetPr>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="113.28515625" customWidth="1"/>
+    <col min="1" max="1" width="113.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="40.5" customHeight="1">
       <c r="A2" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>